<commit_message>
Screen-show repair - funccional atm
</commit_message>
<xml_diff>
--- a/data/chamadas_csv/nova_planilha_ocorrencias.xlsx
+++ b/data/chamadas_csv/nova_planilha_ocorrencias.xlsx
@@ -487,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,7 +2005,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 08:43</t>
+          <t>12/01/2026 11:54</t>
         </is>
       </c>
       <c r="C37" s="7" t="inlineStr">
@@ -2120,6 +2120,216 @@
       <c r="H39" s="3" t="inlineStr">
         <is>
           <t>ASL00063</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 13:06</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 17:38</t>
+        </is>
+      </c>
+      <c r="C40" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>2026-43493193-0</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>P01001 - VISTORIA DE FISCALIZACAO</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr">
+        <is>
+          <t>RUA AURORA, Nº 17 - SAO BENEDITO - PASSOS</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>APV06243</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 14:13</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 14:43</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>2026-43494141-1</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>V02201 - VITIMA DE CHOQUE DE BICICLETA</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="inlineStr">
+        <is>
+          <t>AVENIDA ESTACAO, Nº 210 - PARQUE DA ESTACAO - PASSOS</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 14:23</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 15:32</t>
+        </is>
+      </c>
+      <c r="C42" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>2026-43494289-2</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>V01008 - VITIMA COM DOR ABDOMINAL</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="inlineStr">
+        <is>
+          <t>RUA MISSOES, Nº 565 - JARDIM PLANALTO - PASSOS</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 17:46</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 18:51</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>2026-43498275-0</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="inlineStr">
+        <is>
+          <t>RUA SAGU, Nº 16 - RESIDENCIAL PORTAL DAS PALMEIRAS - PASSOS</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 19:39</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>12/01/2026 19:42</t>
+        </is>
+      </c>
+      <c r="C44" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>2026-43500154-1</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>V01004 - VITIMA COM CRISE DIABETICA / HIPOGLICEMIA</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>RUA ELZO CALIXTO MATTAR, Nº 701 - SANTA RITA - PASSOS</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
automation to get the descriptions
</commit_message>
<xml_diff>
--- a/data/chamadas_csv/nova_planilha_ocorrencias.xlsx
+++ b/data/chamadas_csv/nova_planilha_ocorrencias.xlsx
@@ -86,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -99,6 +99,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -474,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +494,7 @@
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="39" customWidth="1" min="9" max="9"/>
+    <col width="60" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -539,16 +543,21 @@
           <t>Unidade Responsável</t>
         </is>
       </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Histórico</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 17:55</t>
+          <t>17/01/2026 04:19</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 18:51</t>
+          <t>17/01/2026 04:59</t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -563,39 +572,48 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>2026-43563559-8</t>
+          <t>2026-43572413-3</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>V01020 - VITIMA COM PARADA CARDIORRESPIRATORIA</t>
+          <t>V01018 - VITIMA DE MAL NAO DEFINIDO</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>RUA BUENOS AIRES, Nº 433 - PANORAMA - PASSOS</t>
+          <t>RUA MUZAMBINHO, Nº 181 - PASSOS</t>
         </is>
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>ASL00063</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="inlineStr">
+        <is>
+          <t>Descrição
+Solicitante relata que seu filho, 50 anos, encontra-se em tratamento para cirrose
+hepática. Informa que o paciente apresenta dor abdominal, associada a episódios de
+vômito. No momento do chamado, o paciente queixa-se de dor intensa,
+encontrando-se agitado e confuso, com alteração do estado mental.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 17:32</t>
+          <t>16/01/2026 22:44</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 18:13</t>
+          <t>17/01/2026 00:53</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -605,27 +623,27 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>O</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>2026-43563221-1</t>
+          <t>2026-43568437-8</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
+          <t>O02027 - INCENDIO VEIC. AUTOMOTOR</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>RUA AGUAS MARINHAS, Nº 1625 - ACLIMACAO - PASSOS</t>
+          <t>RODOVIA MG 344, Nº S/N - DISTRITO INDUSTRIAL - ITAU DE MINAS</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ABT00816</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
@@ -633,16 +651,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J3" s="5" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 16:27</t>
+          <t>16/01/2026 17:55</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 17:25</t>
+          <t>16/01/2026 18:51</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -657,39 +676,40 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>2026-43562067-8</t>
+          <t>2026-43563559-8</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
+          <t>V01020 - VITIMA COM PARADA CARDIORRESPIRATORIA</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>RUA AGUAS MARINHAS, Nº 1626 - ACLIMACAO - PASSOS</t>
+          <t>RUA BUENOS AIRES, Nº 433 - PANORAMA - PASSOS</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ASL00063</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 15:21</t>
+          <t>16/01/2026 17:32</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 16:50</t>
+          <t>16/01/2026 18:13</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -704,17 +724,17 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>2026-43560863-2</t>
+          <t>2026-43563221-1</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>V01007 - VITIMA COM DISPNEIA</t>
+          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t>RUA SANTO ANIBALE MARIE DI FRANCIA, Nº 28 - CENTRO - PASSOS</t>
+          <t>RUA AGUAS MARINHAS, Nº 1625 - ACLIMACAO - PASSOS</t>
         </is>
       </c>
       <c r="H5" s="3" t="inlineStr">
@@ -727,16 +747,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 15:04</t>
+          <t>16/01/2026 16:27</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 16:32</t>
+          <t>16/01/2026 17:25</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -751,17 +772,17 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>2026-43560533-8</t>
+          <t>2026-43562067-8</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>V02408 - VITIMA DE COLISAO ENTRE AUTOMOVEL X MOTOCICLETA</t>
+          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>RUA PICA PAU / RUA CARAJAS - NOSSA SENHORA APARECIDA - PASSOS</t>
+          <t>RUA AGUAS MARINHAS, Nº 1626 - ACLIMACAO - PASSOS</t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
@@ -774,16 +795,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J6" s="5" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 15:00</t>
+          <t>16/01/2026 15:21</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 16:26</t>
+          <t>16/01/2026 16:50</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -798,39 +820,40 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>2026-43560460-6</t>
+          <t>2026-43560863-2</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>V03008 - VITIMA DE ATAQUE DE CAO</t>
+          <t>V01007 - VITIMA COM DISPNEIA</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA AMAZONAS, Nº 1007 - BELA VISTA 2 - PASSOS</t>
+          <t>RUA SANTO ANIBALE MARIE DI FRANCIA, Nº 28 - CENTRO - PASSOS</t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>ASL00063 / UR04360</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 14:30</t>
+          <t>16/01/2026 15:04</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 15:22</t>
+          <t>16/01/2026 16:32</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -845,17 +868,17 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>2026-43559873-9</t>
+          <t>2026-43560533-8</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>V01009 - VITIMA COM DOR NA COLUNA VERTEBRAL</t>
+          <t>V02408 - VITIMA DE COLISAO ENTRE AUTOMOVEL X MOTOCICLETA</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA JUCA STOCKLER, Nº 984 - BELO HORIZONTE - PASSOS</t>
+          <t>RUA PICA PAU / RUA CARAJAS - NOSSA SENHORA APARECIDA - PASSOS</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
@@ -868,16 +891,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J8" s="5" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 13:40</t>
+          <t>16/01/2026 15:00</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 15:09</t>
+          <t>16/01/2026 16:26</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -887,27 +911,27 @@
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>2026-43559063-9</t>
+          <t>2026-43560460-6</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
+          <t>V03008 - VITIMA DE ATAQUE DE CAO</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>RUA CUBA, Nº 37 - NOVO MUNDO - PASSOS</t>
+          <t>AVENIDA AMAZONAS, Nº 1007 - BELA VISTA 2 - PASSOS</t>
         </is>
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>ASL00063</t>
+          <t>ASL00063 / UR04360</t>
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr">
@@ -915,16 +939,17 @@
           <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
         </is>
       </c>
+      <c r="J9" s="5" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 13:21</t>
+          <t>16/01/2026 14:30</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 14:42</t>
+          <t>16/01/2026 15:22</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
@@ -939,17 +964,17 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>2026-43558853-6</t>
+          <t>2026-43559873-9</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
+          <t>V01009 - VITIMA COM DOR NA COLUNA VERTEBRAL</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>RUA PITANGUI, Nº 363 - COHAB 2 - PASSOS</t>
+          <t>AVENIDA JUCA STOCKLER, Nº 984 - BELO HORIZONTE - PASSOS</t>
         </is>
       </c>
       <c r="H10" s="3" t="inlineStr">
@@ -962,16 +987,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J10" s="5" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 11:37</t>
+          <t>16/01/2026 13:40</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 13:22</t>
+          <t>16/01/2026 21:36</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
@@ -981,44 +1007,45 @@
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>2026-43557828-3</t>
+          <t>2026-43559063-9</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>V01007 - VITIMA COM DISPNEIA</t>
+          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>RUA CORONEL JOAO DE BARROS, Nº 1193 - BELO HORIZONTE - PASSOS</t>
+          <t>RUA CUBA, Nº 37 - NOVO MUNDO - PASSOS</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ASL00063 / ASL07161</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 08:25</t>
+          <t>16/01/2026 13:21</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 19:06</t>
+          <t>16/01/2026 14:42</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
@@ -1028,27 +1055,27 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>2026-43555522-2</t>
+          <t>2026-43558853-6</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>X03000 - EMPENHO ADMINISTRATIVO</t>
+          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
         </is>
       </c>
       <c r="G12" s="3" t="inlineStr">
         <is>
-          <t>RUA DOUTOR CARVALHO, Nº 1455 - NOSSA SENHORA DAS GRAÇAS - PASSOS</t>
+          <t>RUA PITANGUI, Nº 363 - COHAB 2 - PASSOS</t>
         </is>
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>ASL07161</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I12" s="3" t="inlineStr">
@@ -1056,16 +1083,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J12" s="5" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 08:06</t>
+          <t>16/01/2026 11:37</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 09:04</t>
+          <t>16/01/2026 13:22</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -1080,17 +1108,17 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>2026-43555350-9</t>
+          <t>2026-43557828-3</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>V01006 - VITIMA COM DIFICULDADE DE LOCOMOCAO</t>
+          <t>V01007 - VITIMA COM DISPNEIA</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>RUA NITEROI, Nº 1319 - RECANTO DA HARMONIA - PASSOS</t>
+          <t>RUA CORONEL JOAO DE BARROS, Nº 1193 - BELO HORIZONTE - PASSOS</t>
         </is>
       </c>
       <c r="H13" s="3" t="inlineStr">
@@ -1103,63 +1131,65 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J13" s="5" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 07:03</t>
+          <t>16/01/2026 08:25</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>16/01/2026 11:38</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>3ª</t>
+          <t>16/01/2026 19:06</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>X</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>2026-43554842-8</t>
+          <t>2026-43555522-2</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
+          <t>X03000 - EMPENHO ADMINISTRATIVO</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>RUA BARAO DE PASSOS, Nº S/N - SANTA LUZIA - PASSOS</t>
+          <t>RUA DOUTOR CARVALHO, Nº 1455 - NOSSA SENHORA DAS GRAÇAS - PASSOS</t>
         </is>
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>ASL00063</t>
+          <t>ASL07161</t>
         </is>
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J14" s="5" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 20:38</t>
+          <t>16/01/2026 08:06</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 22:03</t>
+          <t>16/01/2026 09:04</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
@@ -1174,7 +1204,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>2026-43501096-2</t>
+          <t>2026-43555350-9</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1184,7 +1214,7 @@
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>RUA QUILOMBO, Nº 532 - CASARAO - PASSOS</t>
+          <t>RUA NITEROI, Nº 1319 - RECANTO DA HARMONIA - PASSOS</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
@@ -1197,63 +1227,65 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J15" s="5" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 19:39</t>
+          <t>16/01/2026 07:03</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 20:43</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>4ª</t>
+          <t>16/01/2026 11:38</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>3ª</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>2026-43500154-1</t>
+          <t>2026-43554842-8</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>V01004 - VITIMA COM CRISE DIABETICA / HIPOGLICEMIA</t>
+          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>RUA ELZO CALIXTO MATTAR, Nº 701 - SANTA RITA - PASSOS</t>
+          <t>RUA BARAO DE PASSOS, Nº S/N - SANTA LUZIA - PASSOS</t>
         </is>
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ASL00063</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J16" s="5" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 17:46</t>
+          <t>12/01/2026 20:38</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 18:51</t>
+          <t>12/01/2026 22:03</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -1268,17 +1300,17 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2026-43498275-0</t>
+          <t>2026-43501096-2</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
+          <t>V01006 - VITIMA COM DIFICULDADE DE LOCOMOCAO</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>RUA SAGU, Nº 16 - RESIDENCIAL PORTAL DAS PALMEIRAS - PASSOS</t>
+          <t>RUA QUILOMBO, Nº 532 - CASARAO - PASSOS</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
@@ -1291,16 +1323,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J17" s="5" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 14:23</t>
+          <t>12/01/2026 19:39</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 15:32</t>
+          <t>12/01/2026 20:43</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
@@ -1315,17 +1348,17 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2026-43494289-2</t>
+          <t>2026-43500154-1</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>V01008 - VITIMA COM DOR ABDOMINAL</t>
+          <t>V01004 - VITIMA COM CRISE DIABETICA / HIPOGLICEMIA</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>RUA MISSOES, Nº 565 - JARDIM PLANALTO - PASSOS</t>
+          <t>RUA ELZO CALIXTO MATTAR, Nº 701 - SANTA RITA - PASSOS</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
@@ -1338,16 +1371,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J18" s="5" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 14:13</t>
+          <t>12/01/2026 17:46</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 14:43</t>
+          <t>12/01/2026 18:51</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -1362,17 +1396,17 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>2026-43494141-1</t>
+          <t>2026-43498275-0</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>V02201 - VITIMA DE CHOQUE DE BICICLETA</t>
+          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA ESTACAO, Nº 210 - PARQUE DA ESTACAO - PASSOS</t>
+          <t>RUA SAGU, Nº 16 - RESIDENCIAL PORTAL DAS PALMEIRAS - PASSOS</t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
@@ -1385,16 +1419,17 @@
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J19" s="5" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 13:06</t>
+          <t>12/01/2026 14:23</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 17:38</t>
+          <t>12/01/2026 15:32</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
@@ -1404,44 +1439,45 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>2026-43493193-0</t>
+          <t>2026-43494289-2</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>P01001 - VISTORIA DE FISCALIZACAO</t>
+          <t>V01008 - VITIMA COM DOR ABDOMINAL</t>
         </is>
       </c>
       <c r="G20" s="3" t="inlineStr">
         <is>
-          <t>RUA AURORA, Nº 17 - SAO BENEDITO - PASSOS</t>
+          <t>RUA MISSOES, Nº 565 - JARDIM PLANALTO - PASSOS</t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>APV06243</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J20" s="5" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 09:41</t>
+          <t>12/01/2026 14:13</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 11:08</t>
+          <t>12/01/2026 14:43</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
@@ -1451,44 +1487,45 @@
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>2026-43490772-0</t>
+          <t>2026-43494141-1</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>S06003 - CAPTURA DE CAO PERIGOSO / AGRESSIVO</t>
+          <t>V02201 - VITIMA DE CHOQUE DE BICICLETA</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
-          <t>RUA LOULOU, Nº 250 - BELO HORIZONTE - PASSOS</t>
+          <t>AVENIDA ESTACAO, Nº 210 - PARQUE DA ESTACAO - PASSOS</t>
         </is>
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>ASL00063</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J21" s="5" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:56</t>
+          <t>12/01/2026 13:06</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 09:08</t>
+          <t>12/01/2026 17:38</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
@@ -1498,49 +1535,50 @@
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>2026-43489573-7</t>
+          <t>2026-43493193-0</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
+          <t>P01001 - VISTORIA DE FISCALIZACAO</t>
         </is>
       </c>
       <c r="G22" s="3" t="inlineStr">
         <is>
-          <t>RUA INDIANA, Nº 1583 - PASSOS</t>
+          <t>RUA AURORA, Nº 17 - SAO BENEDITO - PASSOS</t>
         </is>
       </c>
       <c r="H22" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>APV06243</t>
         </is>
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J22" s="5" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:04</t>
+          <t>12/01/2026 09:41</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 11:54</t>
-        </is>
-      </c>
-      <c r="C23" s="5" t="inlineStr">
-        <is>
-          <t>3ª</t>
+          <t>12/01/2026 11:08</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -1550,44 +1588,45 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>2026-43489174-1</t>
+          <t>2026-43490772-0</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>S06002 - CAPTURA DE ANIMAL SILVESTRE PERIGOSO / AGRESSIVO</t>
+          <t>S06003 - CAPTURA DE CAO PERIGOSO / AGRESSIVO</t>
         </is>
       </c>
       <c r="G23" s="3" t="inlineStr">
         <is>
-          <t>RUA ESPIRITO SANTO, Nº 260 - CENTRO - ALPINOPOLIS</t>
+          <t>RUA LOULOU, Nº 250 - BELO HORIZONTE - PASSOS</t>
         </is>
       </c>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>ASL07161</t>
+          <t>ASL00063</t>
         </is>
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
-        </is>
-      </c>
+          <t>1CIA IND/2CIA/PEL PREV E VIST(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J23" s="5" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 06:42</t>
+          <t>12/01/2026 07:56</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:53</t>
-        </is>
-      </c>
-      <c r="C24" s="5" t="inlineStr">
-        <is>
-          <t>3ª</t>
+          <t>12/01/2026 09:08</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -1597,17 +1636,17 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>2026-43489075-0</t>
+          <t>2026-43489573-7</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>V01005 - VITIMA COM CRISE HIPERTENSIVA/HIPOTENSAO</t>
+          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
         </is>
       </c>
       <c r="G24" s="3" t="inlineStr">
         <is>
-          <t>RUA VITORIA, Nº 445 - JARDIM COLEGIO DE PASSOS - PASSOS</t>
+          <t>RUA INDIANA, Nº 1583 - PASSOS</t>
         </is>
       </c>
       <c r="H24" s="3" t="inlineStr">
@@ -1615,63 +1654,73 @@
           <t>UR04360</t>
         </is>
       </c>
-      <c r="I24" s="3" t="inlineStr"/>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J24" s="5" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 22:10</t>
+          <t>12/01/2026 07:04</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:41</t>
-        </is>
-      </c>
-      <c r="C25" s="5" t="inlineStr">
+          <t>12/01/2026 11:54</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>2026-43485106-0</t>
+          <t>2026-43489174-1</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
+          <t>S06002 - CAPTURA DE ANIMAL SILVESTRE PERIGOSO / AGRESSIVO</t>
         </is>
       </c>
       <c r="G25" s="3" t="inlineStr">
         <is>
-          <t>RUA PINTASSILGO, Nº 215 - NOSSA SENHORA DAS GRAÇAS - PASSOS</t>
+          <t>RUA ESPIRITO SANTO, Nº 260 - CENTRO - ALPINOPOLIS</t>
         </is>
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
-        </is>
-      </c>
-      <c r="I25" s="3" t="inlineStr"/>
+          <t>ASL07161</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J25" s="5" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 19:24</t>
+          <t>12/01/2026 06:42</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:33</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="inlineStr">
+          <t>12/01/2026 07:53</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -1683,38 +1732,39 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>2026-43482164-0</t>
+          <t>2026-43489075-0</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>V01018 - VITIMA DE MAL NAO DEFINIDO</t>
+          <t>V01005 - VITIMA COM CRISE HIPERTENSIVA/HIPOTENSAO</t>
         </is>
       </c>
       <c r="G26" s="3" t="inlineStr">
         <is>
-          <t>RUA DOUTOR CARVALHO, Nº 1455 - NOSSA SENHORA DAS GRAÇAS - PASSOS</t>
+          <t>RUA VITORIA, Nº 445 - JARDIM COLEGIO DE PASSOS - PASSOS</t>
         </is>
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>ASL07161</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr"/>
+      <c r="J26" s="5" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 19:01</t>
+          <t>11/01/2026 22:10</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:34</t>
-        </is>
-      </c>
-      <c r="C27" s="5" t="inlineStr">
+          <t>12/01/2026 07:41</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -1726,17 +1776,17 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>2026-43481771-7</t>
+          <t>2026-43485106-0</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>V01020 - VITIMA COM PARADA CARDIORRESPIRATORIA</t>
+          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
         <is>
-          <t>RUA QUINCA COURA, Nº 20 - SANTA CASA - PASSOS</t>
+          <t>RUA PINTASSILGO, Nº 215 - NOSSA SENHORA DAS GRAÇAS - PASSOS</t>
         </is>
       </c>
       <c r="H27" s="3" t="inlineStr">
@@ -1745,19 +1795,20 @@
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr"/>
+      <c r="J27" s="5" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 14:37</t>
+          <t>11/01/2026 19:24</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:34</t>
-        </is>
-      </c>
-      <c r="C28" s="5" t="inlineStr">
+          <t>12/01/2026 07:33</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -1769,30 +1820,31 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>2026-43477672-1</t>
+          <t>2026-43482164-0</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>V01005 - VITIMA COM CRISE HIPERTENSIVA/HIPOTENSAO</t>
+          <t>V01018 - VITIMA DE MAL NAO DEFINIDO</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
         <is>
-          <t>RUA COIMBRAS, Nº S/N - NOSSA SENHORA DE LOURDES - PASSOS</t>
+          <t>RUA DOUTOR CARVALHO, Nº 1455 - NOSSA SENHORA DAS GRAÇAS - PASSOS</t>
         </is>
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ASL07161</t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr"/>
+      <c r="J28" s="5" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 12:34</t>
+          <t>11/01/2026 19:01</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1800,7 +1852,7 @@
           <t>12/01/2026 07:34</t>
         </is>
       </c>
-      <c r="C29" s="5" t="inlineStr">
+      <c r="C29" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -1812,17 +1864,17 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>2026-43476408-8</t>
+          <t>2026-43481771-7</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>V01018 - VITIMA DE MAL NAO DEFINIDO</t>
+          <t>V01020 - VITIMA COM PARADA CARDIORRESPIRATORIA</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
         <is>
-          <t>RUA GOIAS, Nº 1607 - BELA VISTA - PASSOS</t>
+          <t>RUA QUINCA COURA, Nº 20 - SANTA CASA - PASSOS</t>
         </is>
       </c>
       <c r="H29" s="3" t="inlineStr">
@@ -1831,19 +1883,20 @@
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr"/>
+      <c r="J29" s="5" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 11:38</t>
+          <t>11/01/2026 14:37</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 11:39</t>
-        </is>
-      </c>
-      <c r="C30" s="5" t="inlineStr">
+          <t>12/01/2026 07:34</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -1855,26 +1908,31 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>2026-43475963-3</t>
+          <t>2026-43477672-1</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>V01007 - VITIMA COM DISPNEIA</t>
+          <t>V01005 - VITIMA COM CRISE HIPERTENSIVA/HIPOTENSAO</t>
         </is>
       </c>
       <c r="G30" s="3" t="inlineStr">
         <is>
-          <t>RUA VENEZUELA, Nº 199 - POLIVALENTE - PASSOS</t>
-        </is>
-      </c>
-      <c r="H30" s="3" t="inlineStr"/>
+          <t>RUA COIMBRAS, Nº S/N - NOSSA SENHORA DE LOURDES - PASSOS</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
       <c r="I30" s="3" t="inlineStr"/>
+      <c r="J30" s="5" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 11:28</t>
+          <t>11/01/2026 12:34</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1882,50 +1940,51 @@
           <t>12/01/2026 07:34</t>
         </is>
       </c>
-      <c r="C31" s="5" t="inlineStr">
+      <c r="C31" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>2026-43475892-7</t>
+          <t>2026-43476408-8</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>P03006 - PREVENCAO EM EVENTO RELIGIOSO</t>
+          <t>V01018 - VITIMA DE MAL NAO DEFINIDO</t>
         </is>
       </c>
       <c r="G31" s="3" t="inlineStr">
         <is>
-          <t>PRACA OSVALDO AMERICO DOS REIS, Nº S/N - CENTRO - ALPINOPOLIS</t>
+          <t>RUA GOIAS, Nº 1607 - BELA VISTA - PASSOS</t>
         </is>
       </c>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>BM1550375</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I31" s="3" t="inlineStr"/>
+      <c r="J31" s="5" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 11:06</t>
+          <t>11/01/2026 11:38</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>12/01/2026 07:34</t>
-        </is>
-      </c>
-      <c r="C32" s="5" t="inlineStr">
+          <t>11/01/2026 11:39</t>
+        </is>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -1937,7 +1996,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>2026-43475698-4</t>
+          <t>2026-43475963-3</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
@@ -1947,20 +2006,17 @@
       </c>
       <c r="G32" s="3" t="inlineStr">
         <is>
-          <t>RUA JANAUBA, Nº 156 - COHAB 2 - PASSOS</t>
-        </is>
-      </c>
-      <c r="H32" s="3" t="inlineStr">
-        <is>
-          <t>UR04360</t>
-        </is>
-      </c>
+          <t>RUA VENEZUELA, Nº 199 - POLIVALENTE - PASSOS</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr"/>
       <c r="I32" s="3" t="inlineStr"/>
+      <c r="J32" s="5" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 08:57</t>
+          <t>11/01/2026 11:28</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1968,42 +2024,43 @@
           <t>12/01/2026 07:34</t>
         </is>
       </c>
-      <c r="C33" s="5" t="inlineStr">
+      <c r="C33" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>2026-43474506-6</t>
+          <t>2026-43475892-7</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>V01020 - VITIMA COM PARADA CARDIORRESPIRATORIA</t>
+          <t>P03006 - PREVENCAO EM EVENTO RELIGIOSO</t>
         </is>
       </c>
       <c r="G33" s="3" t="inlineStr">
         <is>
-          <t>RUA PEIXE, Nº 56 - SERRA VERDE - PASSOS</t>
+          <t>PRACA OSVALDO AMERICO DOS REIS, Nº S/N - CENTRO - ALPINOPOLIS</t>
         </is>
       </c>
       <c r="H33" s="3" t="inlineStr">
         <is>
-          <t>ASL07161 / UR04360</t>
+          <t>BM1550375</t>
         </is>
       </c>
       <c r="I33" s="3" t="inlineStr"/>
+      <c r="J33" s="5" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 08:35</t>
+          <t>11/01/2026 11:06</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -2011,7 +2068,7 @@
           <t>12/01/2026 07:34</t>
         </is>
       </c>
-      <c r="C34" s="5" t="inlineStr">
+      <c r="C34" s="6" t="inlineStr">
         <is>
           <t>3ª</t>
         </is>
@@ -2023,7 +2080,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>2026-43474349-0</t>
+          <t>2026-43475698-4</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
@@ -2033,7 +2090,7 @@
       </c>
       <c r="G34" s="3" t="inlineStr">
         <is>
-          <t>RUA ITABIRA, Nº 124 - CALIFORNIA - PASSOS</t>
+          <t>RUA JANAUBA, Nº 156 - COHAB 2 - PASSOS</t>
         </is>
       </c>
       <c r="H34" s="3" t="inlineStr">
@@ -2042,21 +2099,22 @@
         </is>
       </c>
       <c r="I34" s="3" t="inlineStr"/>
+      <c r="J34" s="5" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 23:51</t>
+          <t>11/01/2026 08:57</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 23:52</t>
+          <t>12/01/2026 07:34</t>
         </is>
       </c>
       <c r="C35" s="6" t="inlineStr">
         <is>
-          <t>2ª</t>
+          <t>3ª</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
@@ -2066,36 +2124,41 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>2026-43470020-2</t>
+          <t>2026-43474506-6</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
+          <t>V01020 - VITIMA COM PARADA CARDIORRESPIRATORIA</t>
         </is>
       </c>
       <c r="G35" s="3" t="inlineStr">
         <is>
-          <t>RUA UM - PASSOS</t>
-        </is>
-      </c>
-      <c r="H35" s="3" t="inlineStr"/>
+          <t>RUA PEIXE, Nº 56 - SERRA VERDE - PASSOS</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>ASL07161 / UR04360</t>
+        </is>
+      </c>
       <c r="I35" s="3" t="inlineStr"/>
+      <c r="J35" s="5" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 23:39</t>
+          <t>11/01/2026 08:35</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 06:45</t>
+          <t>12/01/2026 07:34</t>
         </is>
       </c>
       <c r="C36" s="6" t="inlineStr">
         <is>
-          <t>2ª</t>
+          <t>3ª</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -2105,17 +2168,17 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>2026-43469739-5</t>
+          <t>2026-43474349-0</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>V03003 - VITIMA DE AGRESSAO FISICA COM ARMA BRANCA</t>
+          <t>V01007 - VITIMA COM DISPNEIA</t>
         </is>
       </c>
       <c r="G36" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA JUCA STOCKLER, Nº S/N - SAO JOAQUIM - PASSOS</t>
+          <t>RUA ITABIRA, Nº 124 - CALIFORNIA - PASSOS</t>
         </is>
       </c>
       <c r="H36" s="3" t="inlineStr">
@@ -2124,19 +2187,20 @@
         </is>
       </c>
       <c r="I36" s="3" t="inlineStr"/>
+      <c r="J36" s="5" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 22:35</t>
+          <t>10/01/2026 23:51</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 06:45</t>
-        </is>
-      </c>
-      <c r="C37" s="6" t="inlineStr">
+          <t>10/01/2026 23:52</t>
+        </is>
+      </c>
+      <c r="C37" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
@@ -2148,30 +2212,27 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>2026-43468456-5</t>
+          <t>2026-43470020-2</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>V01025 - VITIMA DE USO / ABUSO / DEPENDENCIA DE DROGAS / ALCOOL</t>
+          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
         </is>
       </c>
       <c r="G37" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA ANTONIO ADAO DA SILVA, Nº 719 - COHAB 4 - PASSOS</t>
-        </is>
-      </c>
-      <c r="H37" s="3" t="inlineStr">
-        <is>
-          <t>UR04360</t>
-        </is>
-      </c>
+          <t>RUA UM - PASSOS</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr"/>
       <c r="I37" s="3" t="inlineStr"/>
+      <c r="J37" s="5" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 20:41</t>
+          <t>10/01/2026 23:39</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -2179,7 +2240,7 @@
           <t>11/01/2026 06:45</t>
         </is>
       </c>
-      <c r="C38" s="6" t="inlineStr">
+      <c r="C38" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
@@ -2191,17 +2252,17 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>2026-43466368-9</t>
+          <t>2026-43469739-5</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>V01013 - VITIMA DE EMERGENCIAS PSIQUIATRICAS</t>
+          <t>V03003 - VITIMA DE AGRESSAO FISICA COM ARMA BRANCA</t>
         </is>
       </c>
       <c r="G38" s="3" t="inlineStr">
         <is>
-          <t>RUA GONCALVES DIAS, Nº 544 - CENTRO - PASSOS</t>
+          <t>AVENIDA JUCA STOCKLER, Nº S/N - SAO JOAQUIM - PASSOS</t>
         </is>
       </c>
       <c r="H38" s="3" t="inlineStr">
@@ -2210,19 +2271,20 @@
         </is>
       </c>
       <c r="I38" s="3" t="inlineStr"/>
+      <c r="J38" s="5" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 20:04</t>
+          <t>10/01/2026 22:35</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 20:16</t>
-        </is>
-      </c>
-      <c r="C39" s="6" t="inlineStr">
+          <t>11/01/2026 06:45</t>
+        </is>
+      </c>
+      <c r="C39" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
@@ -2234,26 +2296,31 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>2026-43465696-2</t>
+          <t>2026-43468456-5</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
+          <t>V01025 - VITIMA DE USO / ABUSO / DEPENDENCIA DE DROGAS / ALCOOL</t>
         </is>
       </c>
       <c r="G39" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA ANTONIO ADAO DA SILVA, Nº 111 - PENHA 2 - PASSOS</t>
-        </is>
-      </c>
-      <c r="H39" s="3" t="inlineStr"/>
+          <t>AVENIDA ANTONIO ADAO DA SILVA, Nº 719 - COHAB 4 - PASSOS</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
       <c r="I39" s="3" t="inlineStr"/>
+      <c r="J39" s="5" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 19:33</t>
+          <t>10/01/2026 20:41</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -2261,7 +2328,7 @@
           <t>11/01/2026 06:45</t>
         </is>
       </c>
-      <c r="C40" s="6" t="inlineStr">
+      <c r="C40" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
@@ -2273,17 +2340,17 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>2026-43465179-0</t>
+          <t>2026-43466368-9</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>V01006 - VITIMA COM DIFICULDADE DE LOCOMOCAO</t>
+          <t>V01013 - VITIMA DE EMERGENCIAS PSIQUIATRICAS</t>
         </is>
       </c>
       <c r="G40" s="3" t="inlineStr">
         <is>
-          <t>RUA BOTELHOS, Nº 1061 - NOSSA SENHORA DE FATIMA - PASSOS</t>
+          <t>RUA GONCALVES DIAS, Nº 544 - CENTRO - PASSOS</t>
         </is>
       </c>
       <c r="H40" s="3" t="inlineStr">
@@ -2292,54 +2359,52 @@
         </is>
       </c>
       <c r="I40" s="3" t="inlineStr"/>
+      <c r="J40" s="5" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 19:21</t>
+          <t>10/01/2026 20:04</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 06:45</t>
-        </is>
-      </c>
-      <c r="C41" s="6" t="inlineStr">
+          <t>10/01/2026 20:16</t>
+        </is>
+      </c>
+      <c r="C41" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>2026-43464985-4</t>
+          <t>2026-43465696-2</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>S06001 - SALVAMENTO DE ANIMAL EM RISCO / PERIGO</t>
+          <t>V01003 - VITIMA COM CRISE CONVULSIVA</t>
         </is>
       </c>
       <c r="G41" s="3" t="inlineStr">
         <is>
-          <t>RANCHO PSS0156 - HAVAI - PORTO VELHO - CLAUDIO LUIZ CARDOSO, Nº S/N - PASSOS</t>
-        </is>
-      </c>
-      <c r="H41" s="3" t="inlineStr">
-        <is>
-          <t>ASL07161</t>
-        </is>
-      </c>
+          <t>AVENIDA ANTONIO ADAO DA SILVA, Nº 111 - PENHA 2 - PASSOS</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr"/>
       <c r="I41" s="3" t="inlineStr"/>
+      <c r="J41" s="5" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 17:45</t>
+          <t>10/01/2026 19:33</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -2347,7 +2412,7 @@
           <t>11/01/2026 06:45</t>
         </is>
       </c>
-      <c r="C42" s="6" t="inlineStr">
+      <c r="C42" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
@@ -2359,17 +2424,17 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>2026-43463355-0</t>
+          <t>2026-43465179-0</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>V01025 - VITIMA DE USO / ABUSO / DEPENDENCIA DE DROGAS / ALCOOL</t>
+          <t>V01006 - VITIMA COM DIFICULDADE DE LOCOMOCAO</t>
         </is>
       </c>
       <c r="G42" s="3" t="inlineStr">
         <is>
-          <t>RUA PADRE PIRES, Nº 55 - SAO FRANCISCO - PASSOS</t>
+          <t>RUA BOTELHOS, Nº 1061 - NOSSA SENHORA DE FATIMA - PASSOS</t>
         </is>
       </c>
       <c r="H42" s="3" t="inlineStr">
@@ -2378,11 +2443,12 @@
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr"/>
+      <c r="J42" s="5" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 11:51</t>
+          <t>10/01/2026 19:21</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -2390,42 +2456,43 @@
           <t>11/01/2026 06:45</t>
         </is>
       </c>
-      <c r="C43" s="6" t="inlineStr">
+      <c r="C43" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>2026-43458780-7</t>
+          <t>2026-43464985-4</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>O04011 - INCENDIO EM AREA URBANA NAO PROTEGIDA</t>
+          <t>S06001 - SALVAMENTO DE ANIMAL EM RISCO / PERIGO</t>
         </is>
       </c>
       <c r="G43" s="3" t="inlineStr">
         <is>
-          <t>RUA FARMACEUTICOS, Nº S/N - MONSENHOR MESSIAS - PASSOS</t>
+          <t>RANCHO PSS0156 - HAVAI - PORTO VELHO - CLAUDIO LUIZ CARDOSO, Nº S/N - PASSOS</t>
         </is>
       </c>
       <c r="H43" s="3" t="inlineStr">
         <is>
-          <t>ABT00816</t>
+          <t>ASL07161</t>
         </is>
       </c>
       <c r="I43" s="3" t="inlineStr"/>
+      <c r="J43" s="5" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 11:07</t>
+          <t>10/01/2026 17:45</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -2433,42 +2500,43 @@
           <t>11/01/2026 06:45</t>
         </is>
       </c>
-      <c r="C44" s="6" t="inlineStr">
+      <c r="C44" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>2026-43458335-4</t>
+          <t>2026-43463355-0</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>S06003 - CAPTURA DE CAO PERIGOSO / AGRESSIVO</t>
+          <t>V01025 - VITIMA DE USO / ABUSO / DEPENDENCIA DE DROGAS / ALCOOL</t>
         </is>
       </c>
       <c r="G44" s="3" t="inlineStr">
         <is>
-          <t>RUA CHILE, Nº 520 - POLIVALENTE - PASSOS</t>
+          <t>RUA PADRE PIRES, Nº 55 - SAO FRANCISCO - PASSOS</t>
         </is>
       </c>
       <c r="H44" s="3" t="inlineStr">
         <is>
-          <t>ASL07161</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I44" s="3" t="inlineStr"/>
+      <c r="J44" s="5" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 10:52</t>
+          <t>10/01/2026 11:51</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -2476,95 +2544,97 @@
           <t>11/01/2026 06:45</t>
         </is>
       </c>
-      <c r="C45" s="6" t="inlineStr">
+      <c r="C45" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>O</t>
         </is>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>2026-43458156-5</t>
+          <t>2026-43458780-7</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>V02412 - VITIMA DE COLISAO ENTRE CAMINHAO / CARRETA X MOTOCICLETA</t>
+          <t>O04011 - INCENDIO EM AREA URBANA NAO PROTEGIDA</t>
         </is>
       </c>
       <c r="G45" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA JK, Nº 407 - JARDIM COLEGIO DE PASSOS - PASSOS</t>
+          <t>RUA FARMACEUTICOS, Nº S/N - MONSENHOR MESSIAS - PASSOS</t>
         </is>
       </c>
       <c r="H45" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ABT00816</t>
         </is>
       </c>
       <c r="I45" s="3" t="inlineStr"/>
+      <c r="J45" s="5" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 08:23</t>
+          <t>10/01/2026 11:07</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>11/01/2026 06:46</t>
-        </is>
-      </c>
-      <c r="C46" s="6" t="inlineStr">
+          <t>11/01/2026 06:45</t>
+        </is>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
         <is>
           <t>2ª</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>2026-43456726-0</t>
+          <t>2026-43458335-4</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
+          <t>S06003 - CAPTURA DE CAO PERIGOSO / AGRESSIVO</t>
         </is>
       </c>
       <c r="G46" s="3" t="inlineStr">
         <is>
-          <t>RUA DAVID BALDINI, Nº 71 - CENTRO - PASSOS</t>
+          <t>RUA CHILE, Nº 520 - POLIVALENTE - PASSOS</t>
         </is>
       </c>
       <c r="H46" s="3" t="inlineStr">
         <is>
-          <t>ASL00063 / ABT00816</t>
+          <t>ASL07161</t>
         </is>
       </c>
       <c r="I46" s="3" t="inlineStr"/>
+      <c r="J46" s="5" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 03:38</t>
+          <t>10/01/2026 10:52</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 07:54</t>
+          <t>11/01/2026 06:45</t>
         </is>
       </c>
       <c r="C47" s="7" t="inlineStr">
         <is>
-          <t>1ª</t>
+          <t>2ª</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
@@ -2574,17 +2644,17 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>2026-43455345-1</t>
+          <t>2026-43458156-5</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
+          <t>V02412 - VITIMA DE COLISAO ENTRE CAMINHAO / CARRETA X MOTOCICLETA</t>
         </is>
       </c>
       <c r="G47" s="3" t="inlineStr">
         <is>
-          <t>RUA PITANGAS, Nº 267 - NOVA CALIFORNIA - PASSOS</t>
+          <t>AVENIDA JK, Nº 407 - JARDIM COLEGIO DE PASSOS - PASSOS</t>
         </is>
       </c>
       <c r="H47" s="3" t="inlineStr">
@@ -2593,62 +2663,64 @@
         </is>
       </c>
       <c r="I47" s="3" t="inlineStr"/>
+      <c r="J47" s="5" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 21:38</t>
+          <t>10/01/2026 08:23</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 07:54</t>
+          <t>11/01/2026 06:46</t>
         </is>
       </c>
       <c r="C48" s="7" t="inlineStr">
         <is>
-          <t>1ª</t>
+          <t>2ª</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>2026-43450481-2</t>
+          <t>2026-43456726-0</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>V03008 - VITIMA DE ATAQUE DE CAO</t>
+          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
         </is>
       </c>
       <c r="G48" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA ARLINDO FIGUEIREDO, Nº 462 - CANDEIAS - PASSOS</t>
+          <t>RUA DAVID BALDINI, Nº 71 - CENTRO - PASSOS</t>
         </is>
       </c>
       <c r="H48" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ASL00063 / ABT00816</t>
         </is>
       </c>
       <c r="I48" s="3" t="inlineStr"/>
+      <c r="J48" s="5" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 21:13</t>
+          <t>10/01/2026 03:38</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 21:26</t>
-        </is>
-      </c>
-      <c r="C49" s="7" t="inlineStr">
+          <t>10/01/2026 07:54</t>
+        </is>
+      </c>
+      <c r="C49" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
@@ -2660,77 +2732,83 @@
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>2026-43450039-8</t>
+          <t>2026-43455345-1</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>V01023 - VITIMA DE SINCOPE</t>
+          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
         </is>
       </c>
       <c r="G49" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA DA moda , Nº 2168 - PASSOS</t>
-        </is>
-      </c>
-      <c r="H49" s="3" t="inlineStr"/>
+          <t>RUA PITANGAS, Nº 267 - NOVA CALIFORNIA - PASSOS</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
       <c r="I49" s="3" t="inlineStr"/>
+      <c r="J49" s="5" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 21:09</t>
+          <t>09/01/2026 21:38</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 07:53</t>
-        </is>
-      </c>
-      <c r="C50" s="7" t="inlineStr">
+          <t>10/01/2026 07:54</t>
+        </is>
+      </c>
+      <c r="C50" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>2026-43449969-2</t>
+          <t>2026-43450481-2</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>S06003 - CAPTURA DE CAO PERIGOSO / AGRESSIVO</t>
+          <t>V03008 - VITIMA DE ATAQUE DE CAO</t>
         </is>
       </c>
       <c r="G50" s="3" t="inlineStr">
         <is>
-          <t>RUA JOAO TEIXEIRA MENDES, Nº S/N - FLAMBOYANT - PASSOS</t>
+          <t>AVENIDA ARLINDO FIGUEIREDO, Nº 462 - CANDEIAS - PASSOS</t>
         </is>
       </c>
       <c r="H50" s="3" t="inlineStr">
         <is>
-          <t>ASL07161</t>
+          <t>UR04360</t>
         </is>
       </c>
       <c r="I50" s="3" t="inlineStr"/>
+      <c r="J50" s="5" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 19:02</t>
+          <t>09/01/2026 21:13</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 19:45</t>
-        </is>
-      </c>
-      <c r="C51" s="7" t="inlineStr">
+          <t>09/01/2026 21:26</t>
+        </is>
+      </c>
+      <c r="C51" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
@@ -2742,7 +2820,7 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>2026-43447911-1</t>
+          <t>2026-43450039-8</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
@@ -2752,102 +2830,101 @@
       </c>
       <c r="G51" s="3" t="inlineStr">
         <is>
-          <t>RUA MADRE MARIA DEL VALLE, Nº 65 - CANDEIAS - PASSOS</t>
+          <t>AVENIDA DA moda , Nº 2168 - PASSOS</t>
         </is>
       </c>
       <c r="H51" s="3" t="inlineStr"/>
       <c r="I51" s="3" t="inlineStr"/>
+      <c r="J51" s="5" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 18:17</t>
+          <t>09/01/2026 21:09</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 07:54</t>
-        </is>
-      </c>
-      <c r="C52" s="7" t="inlineStr">
+          <t>10/01/2026 07:53</t>
+        </is>
+      </c>
+      <c r="C52" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>2026-43447129-0</t>
+          <t>2026-43449969-2</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>V02408 - VITIMA DE COLISAO ENTRE AUTOMOVEL X MOTOCICLETA</t>
+          <t>S06003 - CAPTURA DE CAO PERIGOSO / AGRESSIVO</t>
         </is>
       </c>
       <c r="G52" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA PENHA, Nº 94 - PASSOS</t>
+          <t>RUA JOAO TEIXEIRA MENDES, Nº S/N - FLAMBOYANT - PASSOS</t>
         </is>
       </c>
       <c r="H52" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
+          <t>ASL07161</t>
         </is>
       </c>
       <c r="I52" s="3" t="inlineStr"/>
+      <c r="J52" s="5" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 16:44</t>
+          <t>09/01/2026 19:02</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>10/01/2026 07:53</t>
-        </is>
-      </c>
-      <c r="C53" s="7" t="inlineStr">
+          <t>09/01/2026 19:45</t>
+        </is>
+      </c>
+      <c r="C53" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>2026-43445591-1</t>
+          <t>2026-43447911-1</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>P02002 - VISTORIA EM RISCO DE QUEDA DE ARVORE</t>
+          <t>V01023 - VITIMA DE SINCOPE</t>
         </is>
       </c>
       <c r="G53" s="3" t="inlineStr">
         <is>
-          <t>RUA DO MEIO, Nº 270 - NOVO HORIZONTE - PASSOS</t>
-        </is>
-      </c>
-      <c r="H53" s="3" t="inlineStr">
-        <is>
-          <t>ASL07161</t>
-        </is>
-      </c>
+          <t>RUA MADRE MARIA DEL VALLE, Nº 65 - CANDEIAS - PASSOS</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr"/>
       <c r="I53" s="3" t="inlineStr"/>
+      <c r="J53" s="5" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 16:10</t>
+          <t>09/01/2026 18:17</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2855,7 +2932,7 @@
           <t>10/01/2026 07:54</t>
         </is>
       </c>
-      <c r="C54" s="7" t="inlineStr">
+      <c r="C54" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
@@ -2867,7 +2944,7 @@
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>2026-43444998-3</t>
+          <t>2026-43447129-0</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
@@ -2877,7 +2954,7 @@
       </c>
       <c r="G54" s="3" t="inlineStr">
         <is>
-          <t>AVENIDA JK, Nº 800 - BELO HORIZONTE - PASSOS</t>
+          <t>AVENIDA PENHA, Nº 94 - PASSOS</t>
         </is>
       </c>
       <c r="H54" s="3" t="inlineStr">
@@ -2886,11 +2963,12 @@
         </is>
       </c>
       <c r="I54" s="3" t="inlineStr"/>
+      <c r="J54" s="5" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 13:37</t>
+          <t>09/01/2026 16:44</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2898,7 +2976,7 @@
           <t>10/01/2026 07:53</t>
         </is>
       </c>
-      <c r="C55" s="7" t="inlineStr">
+      <c r="C55" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
@@ -2910,17 +2988,17 @@
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>2026-43442356-5</t>
+          <t>2026-43445591-1</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
+          <t>P02002 - VISTORIA EM RISCO DE QUEDA DE ARVORE</t>
         </is>
       </c>
       <c r="G55" s="3" t="inlineStr">
         <is>
-          <t>RUA DAVID BALDINI, Nº 71 - CENTRO - PASSOS</t>
+          <t>RUA DO MEIO, Nº 270 - NOVO HORIZONTE - PASSOS</t>
         </is>
       </c>
       <c r="H55" s="3" t="inlineStr">
@@ -2929,11 +3007,12 @@
         </is>
       </c>
       <c r="I55" s="3" t="inlineStr"/>
+      <c r="J55" s="5" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 11:55</t>
+          <t>09/01/2026 16:10</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2941,7 +3020,7 @@
           <t>10/01/2026 07:54</t>
         </is>
       </c>
-      <c r="C56" s="7" t="inlineStr">
+      <c r="C56" s="8" t="inlineStr">
         <is>
           <t>1ª</t>
         </is>
@@ -2953,17 +3032,17 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>2026-43441344-0</t>
+          <t>2026-43444998-3</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
+          <t>V02408 - VITIMA DE COLISAO ENTRE AUTOMOVEL X MOTOCICLETA</t>
         </is>
       </c>
       <c r="G56" s="3" t="inlineStr">
         <is>
-          <t>RUA CHILE, Nº 177 - POLIVALENTE - PASSOS</t>
+          <t>AVENIDA JK, Nº 800 - BELO HORIZONTE - PASSOS</t>
         </is>
       </c>
       <c r="H56" s="3" t="inlineStr">
@@ -2972,100 +3051,191 @@
         </is>
       </c>
       <c r="I56" s="3" t="inlineStr"/>
+      <c r="J56" s="5" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>08/01/2026 19:29</t>
+          <t>09/01/2026 13:37</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>09/01/2026 08:01</t>
-        </is>
-      </c>
-      <c r="C57" s="4" t="inlineStr">
-        <is>
-          <t>4ª</t>
+          <t>10/01/2026 07:53</t>
+        </is>
+      </c>
+      <c r="C57" s="8" t="inlineStr">
+        <is>
+          <t>1ª</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>2026-43431888-2</t>
+          <t>2026-43442356-5</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>W98011 - SOLICITACAO DE APOIO</t>
+          <t>P02011 - VISTORIA EM ENXAME DE INSETOS</t>
         </is>
       </c>
       <c r="G57" s="3" t="inlineStr">
         <is>
-          <t>RODOVIA BR 146, Nº S/N - DISTRITO INDUSTRIAL 1 - PASSOS</t>
+          <t>RUA DAVID BALDINI, Nº 71 - CENTRO - PASSOS</t>
         </is>
       </c>
       <c r="H57" s="3" t="inlineStr">
         <is>
-          <t>UR04360</t>
-        </is>
-      </c>
-      <c r="I57" s="3" t="inlineStr">
-        <is>
-          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
-        </is>
-      </c>
+          <t>ASL07161</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr"/>
+      <c r="J57" s="5" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
+          <t>09/01/2026 11:55</t>
+        </is>
+      </c>
+      <c r="B58" s="3" t="inlineStr">
+        <is>
+          <t>10/01/2026 07:54</t>
+        </is>
+      </c>
+      <c r="C58" s="8" t="inlineStr">
+        <is>
+          <t>1ª</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>2026-43441344-0</t>
+        </is>
+      </c>
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>V03018 - VITIMA DE QUEDA DA PROPRIA ALTURA</t>
+        </is>
+      </c>
+      <c r="G58" s="3" t="inlineStr">
+        <is>
+          <t>RUA CHILE, Nº 177 - POLIVALENTE - PASSOS</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr"/>
+      <c r="J58" s="5" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>08/01/2026 19:29</t>
+        </is>
+      </c>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>09/01/2026 08:01</t>
+        </is>
+      </c>
+      <c r="C59" s="4" t="inlineStr">
+        <is>
+          <t>4ª</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="inlineStr">
+        <is>
+          <t>2026-43431888-2</t>
+        </is>
+      </c>
+      <c r="F59" s="3" t="inlineStr">
+        <is>
+          <t>W98011 - SOLICITACAO DE APOIO</t>
+        </is>
+      </c>
+      <c r="G59" s="3" t="inlineStr">
+        <is>
+          <t>RODOVIA BR 146, Nº S/N - DISTRITO INDUSTRIAL 1 - PASSOS</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
+        </is>
+      </c>
+      <c r="J59" s="5" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="inlineStr">
+        <is>
           <t>20/07/2025 20:38</t>
         </is>
       </c>
-      <c r="B58" s="3" t="inlineStr">
+      <c r="B60" s="3" t="inlineStr">
         <is>
           <t>21/07/2025 17:39</t>
         </is>
       </c>
-      <c r="C58" s="4" t="inlineStr">
+      <c r="C60" s="4" t="inlineStr">
         <is>
           <t>4ª</t>
         </is>
       </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="E58" s="3" t="inlineStr">
+      <c r="D60" s="3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="inlineStr">
         <is>
           <t>2025-40563281-9</t>
         </is>
       </c>
-      <c r="F58" s="3" t="inlineStr">
+      <c r="F60" s="3" t="inlineStr">
         <is>
           <t>V02102 - VITIMA DE ATROPELAMENTO POR MOTOCICLETA</t>
         </is>
       </c>
-      <c r="G58" s="3" t="inlineStr">
+      <c r="G60" s="3" t="inlineStr">
         <is>
           <t>RUA GERSON RIBEIRO, Nº 270 - NOVA CALIFORNIA - PASSOS</t>
         </is>
       </c>
-      <c r="H58" s="3" t="inlineStr">
-        <is>
-          <t>UR04360</t>
-        </is>
-      </c>
-      <c r="I58" s="3" t="inlineStr">
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>UR04360</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
         <is>
           <t>1CIA IND/2CIA/1PEL(PASSOS)</t>
         </is>
       </c>
+      <c r="J60" s="5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>